<commit_message>
Arquivos JS - Aula sobre DOM
</commit_message>
<xml_diff>
--- a/Modelagem de Dados/Curso de Linguas/Tabela de Dados a serem coletados.xlsx
+++ b/Modelagem de Dados/Curso de Linguas/Tabela de Dados a serem coletados.xlsx
@@ -1,16 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_6C34C163CCB081BD19B6D436355C48C2E22B1BF7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -458,11 +472,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##&quot;/&quot;##&quot;/&quot;####"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,18 +720,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -730,12 +740,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -750,31 +754,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -783,14 +776,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -813,20 +806,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -864,32 +850,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Incorreto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -927,9 +921,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -961,9 +955,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -995,9 +1007,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1170,14 +1200,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
@@ -1196,32 +1226,31 @@
     <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:20">
-      <c r="A4" s="61" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="H4" s="61" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="H4" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1258,26 +1287,25 @@
       <c r="M5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="3"/>
@@ -1295,15 +1323,8 @@
         <v>26</v>
       </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-    </row>
-    <row r="7" spans="1:20">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1314,7 +1335,7 @@
       <c r="D7" s="2">
         <v>50</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="2"/>
@@ -1328,19 +1349,12 @@
       <c r="K7" s="2">
         <v>50</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-    </row>
-    <row r="8" spans="1:20">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -1351,7 +1365,7 @@
       <c r="D8" s="2">
         <v>8</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="2"/>
@@ -1365,13 +1379,12 @@
       <c r="K8" s="2">
         <v>20</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="2"/>
-      <c r="N8" s="28"/>
-    </row>
-    <row r="9" spans="1:20">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -1380,7 +1393,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="2"/>
@@ -1394,13 +1407,13 @@
       <c r="K9" s="2">
         <v>15</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="29"/>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="L9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="22"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -1411,12 +1424,12 @@
       <c r="D10" s="2">
         <v>20</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -1427,20 +1440,20 @@
       <c r="D11" s="2">
         <v>50</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -1449,7 +1462,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="2"/>
@@ -1472,7 +1485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -1487,22 +1500,22 @@
         <v>26</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="12"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -1513,7 +1526,7 @@
       <c r="D14" s="2">
         <v>2</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="2"/>
@@ -1532,7 +1545,7 @@
       </c>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1560,7 +1573,7 @@
       </c>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>32</v>
@@ -1575,15 +1588,15 @@
         <v>27</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="7"/>
-      <c r="P16" s="60"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="6"/>
+      <c r="P16" s="48"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1598,14 +1611,14 @@
         <v>26</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1620,14 +1633,14 @@
         <v>26</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1642,41 +1655,40 @@
         <v>26</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:20" s="64" customFormat="1"/>
-    <row r="21" spans="1:20">
-      <c r="A21" s="61" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="H21" s="61" t="s">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="H21" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="O21" s="61" t="s">
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="O21" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="61"/>
-      <c r="S21" s="61"/>
-      <c r="T21" s="61"/>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1732,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1743,7 +1755,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="2"/>
@@ -1776,7 +1788,7 @@
       </c>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>30</v>
@@ -1787,7 +1799,7 @@
       <c r="D24" s="2">
         <v>50</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="2"/>
@@ -1820,7 +1832,7 @@
       </c>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>34</v>
@@ -1831,7 +1843,7 @@
       <c r="D25" s="2">
         <v>50</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F25" s="2"/>
@@ -1850,7 +1862,7 @@
       </c>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>35</v>
@@ -1880,7 +1892,7 @@
       </c>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>36</v>
@@ -1889,12 +1901,12 @@
         <v>23</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>37</v>
@@ -1905,12 +1917,12 @@
       <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>38</v>
@@ -1926,7 +1938,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
@@ -1942,7 +1954,7 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>33</v>
@@ -1958,7 +1970,7 @@
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>19</v>
       </c>
@@ -1974,26 +1986,26 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:20" s="64" customFormat="1"/>
-    <row r="34" spans="1:20">
-      <c r="A34" s="61" t="s">
+    <row r="33" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="H34" s="61" t="s">
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="H34" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
@@ -2061,7 +2073,7 @@
       </c>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>43</v>
@@ -2089,7 +2101,7 @@
       </c>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>73</v>
@@ -2119,7 +2131,7 @@
       </c>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -2149,13 +2161,13 @@
       </c>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:20">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
         <v>48</v>
@@ -2171,13 +2183,13 @@
       </c>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:20">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
         <v>50</v>
@@ -2193,13 +2205,13 @@
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:20">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
         <v>51</v>
@@ -2215,13 +2227,13 @@
       </c>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:20">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
         <v>52</v>
@@ -2237,13 +2249,13 @@
       </c>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:20">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
         <v>53</v>
@@ -2259,7 +2271,7 @@
       </c>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
         <v>54</v>
@@ -2268,13 +2280,13 @@
         <v>23</v>
       </c>
       <c r="K45" s="2"/>
-      <c r="L45" s="5" t="s">
+      <c r="L45" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M45" s="2"/>
-      <c r="T45" s="60"/>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="T45" s="48"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H46" s="2"/>
       <c r="I46" s="2" t="s">
         <v>55</v>
@@ -2285,12 +2297,12 @@
       <c r="K46" s="2">
         <v>2</v>
       </c>
-      <c r="L46" s="5" t="s">
+      <c r="L46" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H47" s="2"/>
       <c r="I47" s="2" t="s">
         <v>56</v>
@@ -2306,26 +2318,26 @@
       </c>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:20" s="64" customFormat="1"/>
-    <row r="49" spans="1:13">
-      <c r="A49" s="61" t="s">
+    <row r="48" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="61"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="H49" s="61" t="s">
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="H49" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61"/>
-      <c r="M49" s="61"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
@@ -2363,7 +2375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>11</v>
       </c>
@@ -2393,7 +2405,7 @@
       </c>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>59</v>
@@ -2421,7 +2433,7 @@
       </c>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
         <v>60</v>
@@ -2433,7 +2445,7 @@
       <c r="E53" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F53" s="12"/>
+      <c r="F53" s="10"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2" t="s">
         <v>83</v>
@@ -2447,19 +2459,19 @@
       </c>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="12"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="62" t="s">
+      <c r="F54" s="50" t="s">
         <v>80</v>
       </c>
       <c r="H54" s="2"/>
@@ -2475,13 +2487,13 @@
       </c>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="16"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="63"/>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="51"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2" t="s">
         <v>87</v>
@@ -2493,25 +2505,25 @@
       <c r="L55" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M55" s="38" t="s">
+      <c r="M55" s="29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="13" t="s">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" s="13"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="11"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2" t="s">
         <v>84</v>
@@ -2523,11 +2535,11 @@
       <c r="L56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M56" s="17" t="s">
+      <c r="M56" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>19</v>
       </c>
@@ -2538,40 +2550,40 @@
         <v>23</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F57" s="2"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12" t="s">
+      <c r="H57" s="10"/>
+      <c r="I57" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
       <c r="L57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M57" s="17" t="s">
+      <c r="M57" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="18" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H59" s="2" t="s">
         <v>19</v>
       </c>
@@ -2587,7 +2599,7 @@
       </c>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -2595,7 +2607,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2603,37 +2615,37 @@
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="61" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="61"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="30" t="s">
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="30" t="s">
+      <c r="E66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F66" s="30" t="s">
+      <c r="F66" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>11</v>
       </c>
@@ -2644,12 +2656,12 @@
         <v>23</v>
       </c>
       <c r="D67" s="2"/>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
         <v>75</v>
@@ -2660,12 +2672,12 @@
       <c r="D68" s="2">
         <v>50</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
         <v>76</v>
@@ -2681,7 +2693,7 @@
       </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
         <v>77</v>
@@ -2690,12 +2702,12 @@
         <v>23</v>
       </c>
       <c r="D70" s="2"/>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
         <v>78</v>
@@ -2706,12 +2718,12 @@
       <c r="D71" s="2">
         <v>2</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
         <v>79</v>
@@ -2751,14 +2763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:T67"/>
   <sheetViews>
-    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
@@ -2781,103 +2793,103 @@
     <col min="20" max="20" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
-      <c r="B2" s="65" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="Q2" s="66" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="Q2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="68"/>
-    </row>
-    <row r="3" spans="2:20">
-      <c r="B3" s="19" t="s">
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="55"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
-      <c r="B4" s="20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
         <v>54206</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>31051998</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F4" s="2">
         <v>47522031465</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="2">
@@ -2895,20 +2907,20 @@
       <c r="L4" s="2">
         <v>11945652015</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="31">
         <v>234651</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="20">
         <v>100</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="20">
         <v>1000</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="19">
         <f>M4</f>
         <v>234651</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S4" s="2">
@@ -2918,24 +2930,24 @@
         <v>11965654852</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
-      <c r="B5" s="20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
         <f>B4+1</f>
         <v>54207</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>25032001</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="2">
         <v>11025065145</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H5" s="2">
@@ -2953,22 +2965,22 @@
       <c r="L5" s="2">
         <v>11965233256</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5" s="31">
         <f>M4+1</f>
         <v>234652</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="20">
         <v>100</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="20">
         <f>O4+1</f>
         <v>1001</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="19">
         <f>M5</f>
         <v>234652</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>99</v>
       </c>
       <c r="S5" s="2">
@@ -2978,24 +2990,24 @@
         <v>11987564321</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
-      <c r="B6" s="20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
         <f t="shared" ref="B6:B8" si="0">B5+1</f>
         <v>54208</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>14042000</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F6" s="2">
         <v>22053665874</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H6" s="2">
@@ -3013,22 +3025,22 @@
       <c r="L6" s="2">
         <v>11987545623</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6" s="31">
         <f t="shared" ref="M6:M7" si="1">M5+1</f>
         <v>234653</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="20">
         <v>100</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="20">
         <f>O5+1</f>
         <v>1002</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="19">
         <f>M6</f>
         <v>234653</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="5" t="s">
         <v>100</v>
       </c>
       <c r="S6" s="2">
@@ -3038,24 +3050,24 @@
         <v>11965874236</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
-      <c r="B7" s="20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
         <f t="shared" si="0"/>
         <v>54209</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>3041995</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="2">
         <v>15935785245</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H7" s="2">
@@ -3073,22 +3085,22 @@
       <c r="L7" s="2">
         <v>11975369512</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="31">
         <f t="shared" si="1"/>
         <v>234654</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="20">
         <v>100</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="20">
         <f>O6+1</f>
         <v>1003</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="19">
         <f>M7</f>
         <v>234654</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="5" t="s">
         <v>101</v>
       </c>
       <c r="S7" s="2">
@@ -3098,24 +3110,24 @@
         <v>11955498421</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
-      <c r="B8" s="20">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
         <f t="shared" si="0"/>
         <v>54210</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>31051998</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="2">
         <v>45685235725</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H8" s="2">
@@ -3133,22 +3145,22 @@
       <c r="L8" s="2">
         <v>11914521254</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="31">
         <f>M5</f>
         <v>234652</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="20">
         <v>101</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="20">
         <f>O7+1</f>
         <v>1004</v>
       </c>
-      <c r="Q8" s="23">
+      <c r="Q8" s="19">
         <f>Q7+1</f>
         <v>234655</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="5" t="s">
         <v>102</v>
       </c>
       <c r="S8" s="2">
@@ -3158,294 +3170,225 @@
         <v>11923456122</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="22" t="s">
+      <c r="D9" s="8"/>
+      <c r="M9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="2:20">
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="2:20">
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="2:20">
-      <c r="B13" s="61" t="s">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="G13" s="66" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="G13" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="2:20">
-      <c r="B14" s="26" t="s">
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="55"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="2:20">
-      <c r="B15" s="20">
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
         <v>100</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="31">
         <v>1</v>
       </c>
       <c r="D15" s="2">
         <v>10</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="19">
         <v>20</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="33">
         <v>100001</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="33">
         <v>5001</v>
       </c>
-      <c r="J15" s="43">
+      <c r="J15" s="34">
         <v>0.29166666666666669</v>
       </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="2:20">
-      <c r="B16" s="20">
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
         <v>101</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="31">
         <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>12</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="19">
         <v>20</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="33">
         <v>100002</v>
       </c>
-      <c r="I16" s="42">
+      <c r="I16" s="33">
         <v>5001</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="34">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="20">
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
         <v>102</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="35">
         <v>2</v>
       </c>
       <c r="D17" s="2">
         <v>11</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="19">
         <v>21</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="33">
         <v>100001</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="33">
         <v>5001</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="34">
         <v>0.375</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="24" t="s">
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="G18" s="23">
+      <c r="D18" s="37"/>
+      <c r="G18" s="19">
         <v>21</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="33">
         <v>100002</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="33">
         <v>5001</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="34">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="G19" s="24" t="s">
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="45" t="s">
+      <c r="H19" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="61" t="s">
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="M24" s="66" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="M24" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="N24" s="67"/>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="30" t="s">
+      <c r="N24" s="54"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="30" t="s">
+      <c r="J25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="30" t="s">
+      <c r="K25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="30" t="s">
+      <c r="N25" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
-      <c r="B26" s="20">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
         <v>5001</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -3466,25 +3409,25 @@
       <c r="J26" s="2">
         <v>65464621896</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="20">
         <v>500</v>
       </c>
-      <c r="M26" s="20">
+      <c r="M26" s="16">
         <v>100001</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="20">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <f>B26+1</f>
         <v>5002</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -3505,25 +3448,25 @@
       <c r="J27" s="2">
         <v>46464648792</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="20">
         <v>501</v>
       </c>
-      <c r="M27" s="20">
+      <c r="M27" s="16">
         <v>100002</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
-      <c r="B28" s="20">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
         <f t="shared" ref="B28:B29" si="2">B27+1</f>
         <v>5003</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -3544,25 +3487,25 @@
       <c r="J28" s="2">
         <v>35789117846</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="20">
         <v>502</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="16">
         <v>100003</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="20">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
         <f t="shared" si="2"/>
         <v>5004</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -3571,136 +3514,132 @@
       <c r="F29" s="2">
         <v>1420</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="10">
         <v>11954657854</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="10">
         <v>65848653596</v>
       </c>
-      <c r="K29" s="47">
+      <c r="K29" s="38">
         <v>503</v>
       </c>
-      <c r="M29" s="24" t="s">
+      <c r="M29" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
-      <c r="B30" s="24" t="s">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="45" t="s">
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="49"/>
-      <c r="E31" s="50"/>
-    </row>
-    <row r="32" spans="2:14">
-      <c r="E32" s="50"/>
-    </row>
-    <row r="33" spans="2:18">
-      <c r="B33" s="61" t="s">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="28"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="G33" s="61" t="s">
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="G33" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="61"/>
-      <c r="P33" s="61"/>
-      <c r="Q33" s="61"/>
-      <c r="R33" s="61"/>
-    </row>
-    <row r="34" spans="2:18">
-      <c r="B34" s="30" t="s">
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I34" s="30" t="s">
+      <c r="I34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J34" s="30" t="s">
+      <c r="J34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M34" s="30" t="s">
+      <c r="M34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N34" s="30" t="s">
+      <c r="N34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O34" s="30" t="s">
+      <c r="O34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P34" s="30" t="s">
+      <c r="P34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q34" s="30" t="s">
+      <c r="Q34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R34" s="30" t="s">
+      <c r="R34" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="2:18">
-      <c r="B35" s="20">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="16">
         <v>500</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="20">
         <v>10001</v>
       </c>
-      <c r="G35" s="20">
+      <c r="G35" s="16">
         <v>10001</v>
       </c>
-      <c r="H35" s="51">
+      <c r="H35" s="2">
         <v>503</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="5" t="s">
         <v>108</v>
       </c>
       <c r="J35" s="2" t="s">
@@ -3713,10 +3652,10 @@
         <v>1133666152</v>
       </c>
       <c r="M35" s="2"/>
-      <c r="N35" s="52" t="s">
+      <c r="N35" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="O35" s="52" t="s">
+      <c r="O35" s="40" t="s">
         <v>128</v>
       </c>
       <c r="P35" s="2">
@@ -3725,28 +3664,28 @@
       <c r="Q35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="R35" s="52" t="s">
+      <c r="R35" s="40" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="2:18">
-      <c r="B36" s="20">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="16">
         <v>501</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="20">
         <v>10001</v>
       </c>
-      <c r="G36" s="20">
+      <c r="G36" s="16">
         <v>10002</v>
       </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
       <c r="J36" s="2" t="s">
         <v>130</v>
       </c>
@@ -3759,10 +3698,10 @@
       <c r="M36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="N36" s="52" t="s">
+      <c r="N36" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="O36" s="52" t="s">
+      <c r="O36" s="40" t="s">
         <v>134</v>
       </c>
       <c r="P36" s="2">
@@ -3771,110 +3710,107 @@
       <c r="Q36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="R36" s="52" t="s">
+      <c r="R36" s="40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="2:18">
-      <c r="B37" s="20">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="16">
         <v>502</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="20">
         <v>10001</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="2:18">
-      <c r="B38" s="20">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="16">
         <v>503</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>108</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="20">
         <v>10001</v>
       </c>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-    </row>
-    <row r="39" spans="2:18">
-      <c r="B39" s="24" t="s">
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="45" t="s">
+      <c r="E39" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
-      <c r="B50" s="66" t="s">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="68"/>
-      <c r="I50" s="66" t="s">
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="55"/>
+      <c r="I50" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="J50" s="67"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="67"/>
-      <c r="N50" s="68"/>
-    </row>
-    <row r="51" spans="2:14">
-      <c r="B51" s="30" t="s">
+      <c r="J50" s="54"/>
+      <c r="K50" s="54"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="54"/>
+      <c r="N50" s="55"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="C51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="E51" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="32" t="s">
+      <c r="F51" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I51" s="30" t="s">
+      <c r="I51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J51" s="30" t="s">
+      <c r="J51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K51" s="30" t="s">
+      <c r="K51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L51" s="30" t="s">
+      <c r="L51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M51" s="30" t="s">
+      <c r="M51" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N51" s="30" t="s">
+      <c r="N51" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
-      <c r="B52" s="20">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="16">
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -3886,13 +3822,13 @@
       <c r="E52" s="2">
         <v>1600</v>
       </c>
-      <c r="F52" s="40">
+      <c r="F52" s="31">
         <v>20001</v>
       </c>
-      <c r="G52" s="42">
+      <c r="G52" s="33">
         <v>20</v>
       </c>
-      <c r="I52" s="38" t="s">
+      <c r="I52" s="29" t="s">
         <v>93</v>
       </c>
       <c r="J52" s="2" t="s">
@@ -3907,12 +3843,12 @@
       <c r="M52" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="16">
         <v>20001</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
-      <c r="B53" s="20">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="16">
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -3924,16 +3860,16 @@
       <c r="E53" s="2">
         <v>1000</v>
       </c>
-      <c r="F53" s="40">
+      <c r="F53" s="31">
         <v>20001</v>
       </c>
-      <c r="G53" s="42">
+      <c r="G53" s="33">
         <v>21</v>
       </c>
-      <c r="I53" s="53" t="s">
+      <c r="I53" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="J53" s="52" t="s">
+      <c r="J53" s="40" t="s">
         <v>142</v>
       </c>
       <c r="K53" s="2">
@@ -3942,106 +3878,104 @@
       <c r="L53" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M53" s="52" t="s">
+      <c r="M53" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="N53" s="20">
+      <c r="N53" s="16">
         <v>20002</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
-      <c r="B54" s="54">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="42">
         <v>3</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D54" s="10">
         <v>2022</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E54" s="10">
         <v>500</v>
       </c>
-      <c r="F54" s="40">
+      <c r="F54" s="31">
         <v>20001</v>
       </c>
-      <c r="G54" s="42">
+      <c r="G54" s="33">
         <v>22</v>
       </c>
-      <c r="I54" s="8"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="31"/>
-      <c r="N54" s="55"/>
-    </row>
-    <row r="55" spans="2:14">
-      <c r="B55" s="56" t="s">
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="43"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="45" t="s">
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="45" t="s">
+      <c r="G55" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" spans="2:14">
-      <c r="B56" s="31"/>
-    </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="7"/>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="7"/>
-    </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="61" t="s">
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="6"/>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
-      <c r="I60" s="61"/>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="30" t="s">
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F61" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G61" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="H61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I61" s="30" t="s">
+      <c r="I61" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="2:14">
-      <c r="B62" s="20">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="16">
         <v>1000</v>
       </c>
-      <c r="C62" s="25">
+      <c r="C62" s="20">
         <v>100001</v>
       </c>
       <c r="D62" s="2">
@@ -4050,25 +3984,25 @@
       <c r="E62" s="2">
         <v>200</v>
       </c>
-      <c r="F62" s="58">
+      <c r="F62" s="46">
         <f>100-(D62*100/E62)</f>
         <v>94</v>
       </c>
       <c r="G62" s="2">
         <v>7</v>
       </c>
-      <c r="H62" s="58">
+      <c r="H62" s="46">
         <v>1</v>
       </c>
-      <c r="I62" s="25">
+      <c r="I62" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:14">
-      <c r="B63" s="20">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="16">
         <v>1000</v>
       </c>
-      <c r="C63" s="25">
+      <c r="C63" s="20">
         <v>100002</v>
       </c>
       <c r="D63" s="2">
@@ -4077,25 +4011,25 @@
       <c r="E63" s="2">
         <v>150</v>
       </c>
-      <c r="F63" s="58">
+      <c r="F63" s="46">
         <f>100-(D63*100/E63)</f>
         <v>90</v>
       </c>
       <c r="G63" s="2">
         <v>8</v>
       </c>
-      <c r="H63" s="58">
+      <c r="H63" s="46">
         <v>1</v>
       </c>
-      <c r="I63" s="25">
+      <c r="I63" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="20">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="16">
         <v>1000</v>
       </c>
-      <c r="C64" s="25">
+      <c r="C64" s="20">
         <v>100003</v>
       </c>
       <c r="D64" s="2">
@@ -4104,25 +4038,25 @@
       <c r="E64" s="2">
         <v>180</v>
       </c>
-      <c r="F64" s="58">
+      <c r="F64" s="46">
         <f>100-(D64*100/E64)</f>
         <v>87.777777777777771</v>
       </c>
       <c r="G64" s="2">
         <v>3</v>
       </c>
-      <c r="H64" s="59">
+      <c r="H64" s="47">
         <v>2</v>
       </c>
-      <c r="I64" s="25">
+      <c r="I64" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
-      <c r="B65" s="20">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="16">
         <v>1001</v>
       </c>
-      <c r="C65" s="25">
+      <c r="C65" s="20">
         <v>100001</v>
       </c>
       <c r="D65" s="2">
@@ -4131,25 +4065,25 @@
       <c r="E65" s="2">
         <v>200</v>
       </c>
-      <c r="F65" s="58">
+      <c r="F65" s="46">
         <f>100-(D65*100/E65)</f>
         <v>92.5</v>
       </c>
       <c r="G65" s="2">
         <v>10</v>
       </c>
-      <c r="H65" s="58">
+      <c r="H65" s="46">
         <v>1</v>
       </c>
-      <c r="I65" s="25">
+      <c r="I65" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:9">
-      <c r="B66" s="20">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="16">
         <v>1001</v>
       </c>
-      <c r="C66" s="25">
+      <c r="C66" s="20">
         <v>100002</v>
       </c>
       <c r="D66" s="2">
@@ -4158,44 +4092,44 @@
       <c r="E66" s="2">
         <v>133</v>
       </c>
-      <c r="F66" s="58">
+      <c r="F66" s="46">
         <f>100-(D66*100/E66)</f>
         <v>91.729323308270679</v>
       </c>
       <c r="G66" s="2">
         <v>6</v>
       </c>
-      <c r="H66" s="59">
+      <c r="H66" s="47">
         <v>2</v>
       </c>
-      <c r="I66" s="25">
+      <c r="I66" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:9">
-      <c r="B67" s="56" t="s">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="45" t="s">
+      <c r="C67" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I67" s="45" t="s">
+      <c r="I67" s="36" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="G33:R33"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="I50:N50"/>
-    <mergeCell ref="B60:I60"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="M24:N24"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="G33:R33"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="I50:N50"/>
+    <mergeCell ref="B60:I60"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>